<commit_message>
minor changes about renaming tips
</commit_message>
<xml_diff>
--- a/R/Projects_2017/Portugal_David/results.xlsx
+++ b/R/Projects_2017/Portugal_David/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="10 yrs Old_ConnectNearBy" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Nodes</t>
   </si>
@@ -71,6 +71,21 @@
   </si>
   <si>
     <t>Full with maxy yrs Old</t>
+  </si>
+  <si>
+    <t>leaves</t>
+  </si>
+  <si>
+    <t>intern_br_sim</t>
+  </si>
+  <si>
+    <t>intern_br_true</t>
+  </si>
+  <si>
+    <t>diff.tree/2*intern_br_sim</t>
+  </si>
+  <si>
+    <t>diff.tree/2*intern_br_all</t>
   </si>
 </sst>
 </file>
@@ -86,6 +101,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -107,6 +123,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,8 +200,8 @@
   </sheetPr>
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1180,7 +1197,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1193,20 +1210,312 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.015306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.48</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
results baseline and diff seed 2
</commit_message>
<xml_diff>
--- a/R/Projects_2017/Portugal_David/results.xlsx
+++ b/R/Projects_2017/Portugal_David/results.xlsx
@@ -5,19 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="10 yrs Old_ConnectNearBy" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Full " sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="diff_sampling" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="baseline_sampling" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="30">
   <si>
     <t>Nodes</t>
   </si>
@@ -86,6 +88,27 @@
   </si>
   <si>
     <t>diff.tree/2*intern_br_all</t>
+  </si>
+  <si>
+    <t>true_full</t>
+  </si>
+  <si>
+    <t>50 / 49</t>
+  </si>
+  <si>
+    <t>55 / 54</t>
+  </si>
+  <si>
+    <t>60 / 59</t>
+  </si>
+  <si>
+    <t>65 / 64</t>
+  </si>
+  <si>
+    <t>70 / 69</t>
+  </si>
+  <si>
+    <t>72 / 71</t>
   </si>
 </sst>
 </file>
@@ -200,8 +223,8 @@
   </sheetPr>
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1212,7 +1235,7 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1521,4 +1544,1900 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>0.223</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>0.307</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2.322</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1.099</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>8.933</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0.621</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>-0.528</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.436</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2.057</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.633</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.985</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0.452</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>-0.443</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0.8493</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1.626</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.726</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.726</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>227</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>386</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>15.44</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0.308</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>-0.324</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.287</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0.8792</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1.815</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.798</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>304</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>476</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>15.86</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>0.465</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>-0.569</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.356</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0.8014</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.4571</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2.125</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.372</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>193</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>696</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>19.88</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>0.407</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>-0.553</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.319</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>0.8135</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1.635</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.449</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>412</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>526</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>968</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>24.2</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>0.252</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>-0.341</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0.8429</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.5111</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1.845</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.416</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>520</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>650</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>266</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>1260</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>0.308</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>-0.496</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.353</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0.8306</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.56</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1.709</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.377</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.939</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>751</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>302</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>1620</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>32.4</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>-0.592</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.263</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0.8519</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.6727</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1.743</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.217</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>618</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>786</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>349</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>1910</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>34.72</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>-0.551</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>0.8519</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.9166</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1.518</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.964</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>694</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>884</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>476</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>2266</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>37.766</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>0.351</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>-0.659</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>0.332</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>0.8465</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.9384</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1.557</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.069</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.959</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>767</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>977</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>447</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>2758</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>42.43</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>-0.684</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0.343</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>0.8415</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.9857</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1.551</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>830</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1064</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>462</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>3316</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>47.37</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>-0.684</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>0.251</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>0.8618</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.9859</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>916</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1156</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>505</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>3458</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>48.02</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>0.327</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>-0.684</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0.266</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>0.8539</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>0.388</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0.777</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2.015</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>5.06</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0.343</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>-0.164</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.418</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0.8048</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1.734</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1.363</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>-0.276</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0.8939</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2.404</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.955</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.867</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>-1.112</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.579</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.266</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2.374</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>251</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>292</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>9.733</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>0.899</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>-0.906</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.424</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0.7563</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.2857</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1.855</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1.058</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.909</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>336</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>0.668</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>-0.575</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.498</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>0.7655</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2.007</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.697</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.983</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>288</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>408</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>248</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>506</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>12.65</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>0.677</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>-0.744</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0.402</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0.7675</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.355</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2.061</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>302</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>670</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>14.88</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>0.603</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>-0.715</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.398</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0.7657</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.4897</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1.685</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>374</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>538</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>336</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>834</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>16.68</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>-0.616</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.428</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0.7682</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1.833</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.984</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>523</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>701</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>385</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>990</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>0.791</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>-0.129</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>0.438</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>0.7741</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.7796</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0.214</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>801</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>463</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>1316</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>21.933</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>0.702</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>-1.092</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>0.7737</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.7968</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1.558</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.264</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.983</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>755</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>967</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>467</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>1680</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>25.84</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>-0.736</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0.447</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>0.7897</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.971</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1.612</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.965</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>883</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1113</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>483</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>2098</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>29.97</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>0.411</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>-0.66</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>0.438</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>0.8011</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.9859</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>916</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1156</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>238</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>574</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>2236</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>0.425</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>-0.699</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0.437</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>0.8034</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>